<commit_message>
verifikován osobní odběr CZ
</commit_message>
<xml_diff>
--- a/Doprava a platba - texty pro mail.xlsx
+++ b/Doprava a platba - texty pro mail.xlsx
@@ -354,7 +354,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -374,6 +374,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -381,10 +384,10 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -691,7 +694,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:E3"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,53 +711,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8" t="s">
+      <c r="C1" s="9"/>
+      <c r="D1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8" t="s">
+      <c r="E1" s="9"/>
+      <c r="F1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="8"/>
+      <c r="G1" s="9"/>
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8" t="s">
+      <c r="C2" s="9"/>
+      <c r="D2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8" t="s">
+      <c r="E2" s="9"/>
+      <c r="F2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="8"/>
+      <c r="G2" s="9"/>
     </row>
     <row r="3" spans="1:8" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="7"/>
+      <c r="C3" s="8"/>
       <c r="D3" s="10" t="s">
         <v>25</v>
       </c>
       <c r="E3" s="10"/>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="3" t="s">
+      <c r="G3" s="8"/>
+      <c r="H3" s="11" t="s">
         <v>15</v>
       </c>
     </row>
@@ -762,18 +765,18 @@
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7" t="s">
+      <c r="C4" s="8"/>
+      <c r="D4" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7" t="s">
+      <c r="E4" s="8"/>
+      <c r="F4" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="7"/>
+      <c r="G4" s="8"/>
       <c r="H4" s="3" t="s">
         <v>15</v>
       </c>
@@ -782,18 +785,18 @@
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7" t="s">
+      <c r="C5" s="8"/>
+      <c r="D5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7" t="s">
+      <c r="E5" s="8"/>
+      <c r="F5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="7"/>
+      <c r="G5" s="8"/>
       <c r="H5" s="3" t="s">
         <v>15</v>
       </c>
@@ -802,18 +805,18 @@
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7" t="s">
+      <c r="C6" s="8"/>
+      <c r="D6" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7" t="s">
+      <c r="E6" s="8"/>
+      <c r="F6" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="7"/>
+      <c r="G6" s="8"/>
       <c r="H6" s="3" t="s">
         <v>15</v>
       </c>
@@ -846,7 +849,7 @@
       <c r="B8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="7" t="s">
         <v>32</v>
       </c>
       <c r="D8" s="6" t="s">
@@ -875,20 +878,24 @@
       <c r="C9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7" t="s">
+      <c r="E9" s="8"/>
+      <c r="F9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="7"/>
+      <c r="G9" s="8"/>
       <c r="H9" s="6" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
@@ -905,10 +912,6 @@
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F4:G4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
verifikace objednávky dobírka CZ velkoobchod
</commit_message>
<xml_diff>
--- a/Doprava a platba - texty pro mail.xlsx
+++ b/Doprava a platba - texty pro mail.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Homer\Documents\horejsidoc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="135" windowWidth="19320" windowHeight="12270"/>
   </bookViews>
@@ -377,17 +382,17 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -400,12 +405,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv systému Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv Office">
   <a:themeElements>
     <a:clrScheme name="Kancelář">
       <a:dk1>
@@ -447,7 +455,7 @@
     </a:clrScheme>
     <a:fontScheme name="Kancelář">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -482,7 +490,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -694,7 +702,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="B4" sqref="B4:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -711,53 +719,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9" t="s">
+      <c r="C1" s="11"/>
+      <c r="D1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9" t="s">
+      <c r="E1" s="11"/>
+      <c r="F1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="9"/>
+      <c r="G1" s="11"/>
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9" t="s">
+      <c r="C2" s="11"/>
+      <c r="D2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9" t="s">
+      <c r="E2" s="11"/>
+      <c r="F2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="9"/>
+      <c r="G2" s="11"/>
     </row>
     <row r="3" spans="1:8" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="10" t="s">
+      <c r="C3" s="10"/>
+      <c r="D3" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="8" t="s">
+      <c r="E3" s="9"/>
+      <c r="F3" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="8"/>
-      <c r="H3" s="11" t="s">
+      <c r="G3" s="10"/>
+      <c r="H3" s="8" t="s">
         <v>15</v>
       </c>
     </row>
@@ -765,18 +773,18 @@
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8" t="s">
+      <c r="C4" s="10"/>
+      <c r="D4" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8" t="s">
+      <c r="E4" s="10"/>
+      <c r="F4" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="8"/>
+      <c r="G4" s="10"/>
       <c r="H4" s="3" t="s">
         <v>15</v>
       </c>
@@ -785,18 +793,18 @@
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8" t="s">
+      <c r="C5" s="9"/>
+      <c r="D5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8" t="s">
+      <c r="E5" s="10"/>
+      <c r="F5" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="8"/>
+      <c r="G5" s="10"/>
       <c r="H5" s="3" t="s">
         <v>15</v>
       </c>
@@ -805,18 +813,18 @@
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8" t="s">
+      <c r="C6" s="10"/>
+      <c r="D6" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8" t="s">
+      <c r="E6" s="10"/>
+      <c r="F6" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="8"/>
+      <c r="G6" s="10"/>
       <c r="H6" s="3" t="s">
         <v>15</v>
       </c>
@@ -878,25 +886,20 @@
       <c r="C9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8" t="s">
+      <c r="E9" s="10"/>
+      <c r="F9" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="8"/>
+      <c r="G9" s="10"/>
       <c r="H9" s="6" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="B3:C3"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
@@ -912,6 +915,11 @@
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="B3:C3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add kalkulace objednávky vzor.xlsx
</commit_message>
<xml_diff>
--- a/Doprava a platba - texty pro mail.xlsx
+++ b/Doprava a platba - texty pro mail.xlsx
@@ -385,10 +385,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
@@ -702,7 +702,10 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C4"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="B5" sqref="B5:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -757,10 +760,10 @@
         <v>23</v>
       </c>
       <c r="C3" s="10"/>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="9"/>
+      <c r="E3" s="10"/>
       <c r="F3" s="10" t="s">
         <v>24</v>
       </c>
@@ -777,14 +780,14 @@
         <v>21</v>
       </c>
       <c r="C4" s="10"/>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10" t="s">
+      <c r="E4" s="9"/>
+      <c r="F4" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="10"/>
+      <c r="G4" s="9"/>
       <c r="H4" s="3" t="s">
         <v>15</v>
       </c>
@@ -793,18 +796,18 @@
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="10" t="s">
+      <c r="C5" s="10"/>
+      <c r="D5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10" t="s">
+      <c r="E5" s="9"/>
+      <c r="F5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="10"/>
+      <c r="G5" s="9"/>
       <c r="H5" s="3" t="s">
         <v>15</v>
       </c>
@@ -813,18 +816,18 @@
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10" t="s">
+      <c r="C6" s="9"/>
+      <c r="D6" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10" t="s">
+      <c r="E6" s="9"/>
+      <c r="F6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="10"/>
+      <c r="G6" s="9"/>
       <c r="H6" s="3" t="s">
         <v>15</v>
       </c>
@@ -900,9 +903,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="F9:G9"/>
     <mergeCell ref="B2:C2"/>
@@ -920,6 +920,9 @@
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>